<commit_message>
termine el filtro de fechas
</commit_message>
<xml_diff>
--- a/excel/calendario-v1.xlsx
+++ b/excel/calendario-v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uredu-my.sharepoint.com/personal/luisfe_moreno_urosario_edu_co/Documents/calendario academico 2020 nuevo diseño/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{16003727-C6EF-4AB6-81B8-B898A4348C8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{57814D08-E298-43AE-B1F2-BCFDA69DDA81}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{16003727-C6EF-4AB6-81B8-B898A4348C8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9D8AEA46-3F9F-4231-996F-AD43401C0DBB}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2554,11 +2554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:S268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I139" sqref="I139"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2611,7 +2610,7 @@
       </c>
       <c r="S1" s="18"/>
     </row>
-    <row r="2" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2640,7 +2639,7 @@
       </c>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -2669,7 +2668,7 @@
       </c>
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2696,7 +2695,7 @@
       <c r="J4" s="4"/>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2724,7 +2723,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -2752,7 +2751,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -2780,7 +2779,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2808,7 +2807,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -2836,7 +2835,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -2864,7 +2863,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -2896,7 +2895,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -2928,7 +2927,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
@@ -2960,7 +2959,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -2992,7 +2991,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
@@ -3024,7 +3023,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
@@ -3056,7 +3055,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -3088,7 +3087,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>5</v>
       </c>
@@ -3120,7 +3119,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
@@ -3148,7 +3147,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>4</v>
       </c>
@@ -3176,7 +3175,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
@@ -3204,7 +3203,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
@@ -3232,7 +3231,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>6</v>
       </c>
@@ -3260,7 +3259,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>4</v>
       </c>
@@ -3288,7 +3287,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>4</v>
       </c>
@@ -3316,7 +3315,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>6</v>
       </c>
@@ -3344,7 +3343,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>4</v>
       </c>
@@ -3372,7 +3371,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>4</v>
       </c>
@@ -3400,7 +3399,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
@@ -3428,7 +3427,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>6</v>
       </c>
@@ -3456,7 +3455,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>4</v>
       </c>
@@ -3484,7 +3483,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>6</v>
       </c>
@@ -3512,7 +3511,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>4</v>
       </c>
@@ -3540,7 +3539,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>4</v>
       </c>
@@ -3568,7 +3567,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>4</v>
       </c>
@@ -3596,7 +3595,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>6</v>
       </c>
@@ -3624,7 +3623,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>6</v>
       </c>
@@ -3652,7 +3651,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>4</v>
       </c>
@@ -3680,7 +3679,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>4</v>
       </c>
@@ -3708,7 +3707,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>4</v>
       </c>
@@ -3736,7 +3735,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>4</v>
       </c>
@@ -3764,7 +3763,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>4</v>
       </c>
@@ -3792,7 +3791,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>4</v>
       </c>
@@ -3820,7 +3819,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>7</v>
       </c>
@@ -3852,7 +3851,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>7</v>
       </c>
@@ -3884,7 +3883,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>5</v>
       </c>
@@ -3916,7 +3915,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>5</v>
       </c>
@@ -3948,7 +3947,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>5</v>
       </c>
@@ -3980,7 +3979,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>5</v>
       </c>
@@ -4012,7 +4011,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>8</v>
       </c>
@@ -4044,7 +4043,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>8</v>
       </c>
@@ -4076,7 +4075,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>5</v>
       </c>
@@ -4108,7 +4107,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>5</v>
       </c>
@@ -4140,7 +4139,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>8</v>
       </c>
@@ -4172,7 +4171,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>8</v>
       </c>
@@ -4204,7 +4203,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>5</v>
       </c>
@@ -4236,7 +4235,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>5</v>
       </c>
@@ -4268,7 +4267,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>5</v>
       </c>
@@ -4300,7 +4299,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>5</v>
       </c>
@@ -4332,7 +4331,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>5</v>
       </c>
@@ -4364,7 +4363,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>5</v>
       </c>
@@ -4396,7 +4395,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>5</v>
       </c>
@@ -4428,7 +4427,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>5</v>
       </c>
@@ -4460,7 +4459,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>5</v>
       </c>
@@ -4492,7 +4491,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>5</v>
       </c>
@@ -4524,7 +4523,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>5</v>
       </c>
@@ -4556,7 +4555,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>4</v>
       </c>
@@ -4584,7 +4583,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>4</v>
       </c>
@@ -4612,7 +4611,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>4</v>
       </c>
@@ -4640,7 +4639,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>5</v>
       </c>
@@ -4672,7 +4671,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>5</v>
       </c>
@@ -4704,7 +4703,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>5</v>
       </c>
@@ -4736,7 +4735,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>5</v>
       </c>
@@ -4768,7 +4767,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>5</v>
       </c>
@@ -4800,7 +4799,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>5</v>
       </c>
@@ -4832,7 +4831,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>5</v>
       </c>
@@ -4864,7 +4863,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>5</v>
       </c>
@@ -4896,7 +4895,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>5</v>
       </c>
@@ -4928,7 +4927,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>8</v>
       </c>
@@ -4960,7 +4959,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>5</v>
       </c>
@@ -4992,7 +4991,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>8</v>
       </c>
@@ -5024,7 +5023,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>5</v>
       </c>
@@ -5056,7 +5055,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>5</v>
       </c>
@@ -5088,7 +5087,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>5</v>
       </c>
@@ -5120,7 +5119,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>8</v>
       </c>
@@ -5152,7 +5151,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>5</v>
       </c>
@@ -5184,7 +5183,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>8</v>
       </c>
@@ -5216,7 +5215,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>8</v>
       </c>
@@ -5248,7 +5247,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>8</v>
       </c>
@@ -5280,7 +5279,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>8</v>
       </c>
@@ -5312,7 +5311,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>8</v>
       </c>
@@ -5344,7 +5343,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>8</v>
       </c>
@@ -5376,7 +5375,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>8</v>
       </c>
@@ -5408,7 +5407,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>8</v>
       </c>
@@ -5440,7 +5439,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>8</v>
       </c>
@@ -5472,7 +5471,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>8</v>
       </c>
@@ -5504,7 +5503,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>8</v>
       </c>
@@ -5536,7 +5535,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>5</v>
       </c>
@@ -5568,7 +5567,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>5</v>
       </c>
@@ -5600,7 +5599,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>5</v>
       </c>
@@ -5632,7 +5631,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>5</v>
       </c>
@@ -5664,7 +5663,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>5</v>
       </c>
@@ -5696,7 +5695,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>5</v>
       </c>
@@ -5728,7 +5727,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>5</v>
       </c>
@@ -5760,7 +5759,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>4</v>
       </c>
@@ -5788,7 +5787,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>5</v>
       </c>
@@ -5820,7 +5819,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>4</v>
       </c>
@@ -5848,7 +5847,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>5</v>
       </c>
@@ -5880,7 +5879,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>5</v>
       </c>
@@ -5912,7 +5911,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>5</v>
       </c>
@@ -5944,7 +5943,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>5</v>
       </c>
@@ -5976,7 +5975,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>5</v>
       </c>
@@ -6008,7 +6007,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>5</v>
       </c>
@@ -6040,7 +6039,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="114" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>9</v>
       </c>
@@ -6068,7 +6067,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>9</v>
       </c>
@@ -6096,7 +6095,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>9</v>
       </c>
@@ -6124,7 +6123,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>9</v>
       </c>
@@ -6152,7 +6151,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>9</v>
       </c>
@@ -6180,7 +6179,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>9</v>
       </c>
@@ -6208,7 +6207,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>9</v>
       </c>
@@ -6236,7 +6235,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>9</v>
       </c>
@@ -6264,7 +6263,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>9</v>
       </c>
@@ -6292,7 +6291,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>9</v>
       </c>
@@ -6320,7 +6319,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="124" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>5</v>
       </c>
@@ -6352,7 +6351,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="125" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>9</v>
       </c>
@@ -6380,7 +6379,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="126" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>9</v>
       </c>
@@ -6408,7 +6407,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>9</v>
       </c>
@@ -6436,7 +6435,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="128" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>9</v>
       </c>
@@ -6464,7 +6463,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>9</v>
       </c>
@@ -6492,7 +6491,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="130" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>9</v>
       </c>
@@ -6520,7 +6519,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>9</v>
       </c>
@@ -6548,7 +6547,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>9</v>
       </c>
@@ -6576,7 +6575,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>9</v>
       </c>
@@ -6604,7 +6603,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>7</v>
       </c>
@@ -6636,7 +6635,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>4</v>
       </c>
@@ -6664,7 +6663,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>7</v>
       </c>
@@ -6696,7 +6695,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>7</v>
       </c>
@@ -6728,7 +6727,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>4</v>
       </c>
@@ -6968,7 +6967,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="146" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>5</v>
       </c>
@@ -7000,7 +6999,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>8</v>
       </c>
@@ -7032,7 +7031,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="148" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>8</v>
       </c>
@@ -7064,7 +7063,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="149" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>8</v>
       </c>
@@ -7096,7 +7095,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="150" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>8</v>
       </c>
@@ -7128,7 +7127,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="151" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>5</v>
       </c>
@@ -7160,7 +7159,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="152" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>5</v>
       </c>
@@ -7192,7 +7191,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="153" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>8</v>
       </c>
@@ -7224,7 +7223,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="154" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>8</v>
       </c>
@@ -7256,7 +7255,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="155" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>8</v>
       </c>
@@ -7288,7 +7287,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="156" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>8</v>
       </c>
@@ -7320,7 +7319,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="157" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>8</v>
       </c>
@@ -7352,7 +7351,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="158" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>8</v>
       </c>
@@ -7384,7 +7383,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="159" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>8</v>
       </c>
@@ -7416,7 +7415,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="160" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>5</v>
       </c>
@@ -7448,7 +7447,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>5</v>
       </c>
@@ -7480,7 +7479,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>5</v>
       </c>
@@ -7512,7 +7511,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>8</v>
       </c>
@@ -7544,7 +7543,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>8</v>
       </c>
@@ -7576,7 +7575,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>8</v>
       </c>
@@ -7608,7 +7607,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>8</v>
       </c>
@@ -7640,7 +7639,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>8</v>
       </c>
@@ -7672,7 +7671,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>5</v>
       </c>
@@ -7704,7 +7703,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>5</v>
       </c>
@@ -7736,7 +7735,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>5</v>
       </c>
@@ -7768,7 +7767,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>5</v>
       </c>
@@ -7800,7 +7799,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>5</v>
       </c>
@@ -7832,7 +7831,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>5</v>
       </c>
@@ -7864,7 +7863,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>5</v>
       </c>
@@ -7896,7 +7895,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>5</v>
       </c>
@@ -7928,7 +7927,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="176" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>5</v>
       </c>
@@ -7960,7 +7959,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="177" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>5</v>
       </c>
@@ -7992,7 +7991,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="178" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>5</v>
       </c>
@@ -8024,7 +8023,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="179" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>5</v>
       </c>
@@ -8056,7 +8055,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="180" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>8</v>
       </c>
@@ -8088,7 +8087,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="181" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>5</v>
       </c>
@@ -8120,7 +8119,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="182" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>5</v>
       </c>
@@ -8152,7 +8151,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="183" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>8</v>
       </c>
@@ -8184,7 +8183,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="184" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>5</v>
       </c>
@@ -8216,7 +8215,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="185" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>5</v>
       </c>
@@ -8248,7 +8247,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="186" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>5</v>
       </c>
@@ -8280,7 +8279,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="187" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>5</v>
       </c>
@@ -8312,7 +8311,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="188" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>6</v>
       </c>
@@ -8340,7 +8339,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="189" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>6</v>
       </c>
@@ -8368,7 +8367,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="190" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>5</v>
       </c>
@@ -8400,7 +8399,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="191" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>5</v>
       </c>
@@ -8432,7 +8431,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="192" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>5</v>
       </c>
@@ -8464,7 +8463,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="193" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>5</v>
       </c>
@@ -8496,7 +8495,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="194" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>5</v>
       </c>
@@ -8528,7 +8527,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="195" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>5</v>
       </c>
@@ -8560,7 +8559,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="196" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>5</v>
       </c>
@@ -8592,7 +8591,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="197" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>5</v>
       </c>
@@ -8624,7 +8623,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="198" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>5</v>
       </c>
@@ -8656,7 +8655,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="199" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>6</v>
       </c>
@@ -8684,7 +8683,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="200" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>6</v>
       </c>
@@ -8712,7 +8711,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="201" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>6</v>
       </c>
@@ -8740,7 +8739,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="202" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>5</v>
       </c>
@@ -8772,7 +8771,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="203" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>5</v>
       </c>
@@ -8804,7 +8803,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="204" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>5</v>
       </c>
@@ -8836,7 +8835,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="205" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>5</v>
       </c>
@@ -8868,7 +8867,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="206" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>5</v>
       </c>
@@ -8900,7 +8899,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="207" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>5</v>
       </c>
@@ -8932,7 +8931,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="208" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>5</v>
       </c>
@@ -8964,7 +8963,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="209" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>5</v>
       </c>
@@ -8996,7 +8995,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="210" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>5</v>
       </c>
@@ -9028,7 +9027,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="211" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>5</v>
       </c>
@@ -9060,7 +9059,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="212" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>5</v>
       </c>
@@ -9092,7 +9091,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="213" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>5</v>
       </c>
@@ -9124,7 +9123,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="214" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>5</v>
       </c>
@@ -9156,7 +9155,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="215" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>5</v>
       </c>
@@ -9188,7 +9187,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="216" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>8</v>
       </c>
@@ -9220,7 +9219,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="217" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>8</v>
       </c>
@@ -9252,7 +9251,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="218" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>8</v>
       </c>
@@ -9284,7 +9283,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="219" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>8</v>
       </c>
@@ -9316,7 +9315,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>8</v>
       </c>
@@ -9348,7 +9347,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>8</v>
       </c>
@@ -9380,7 +9379,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>8</v>
       </c>
@@ -9412,7 +9411,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="223" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>5</v>
       </c>
@@ -9444,7 +9443,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="224" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>5</v>
       </c>
@@ -9476,7 +9475,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="225" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>5</v>
       </c>
@@ -9508,7 +9507,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="226" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>5</v>
       </c>
@@ -9540,7 +9539,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="227" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>5</v>
       </c>
@@ -9572,7 +9571,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="228" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>8</v>
       </c>
@@ -9604,7 +9603,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="229" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>10</v>
       </c>
@@ -9636,7 +9635,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="230" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>8</v>
       </c>
@@ -9668,7 +9667,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="231" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>8</v>
       </c>
@@ -9700,7 +9699,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="232" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>8</v>
       </c>
@@ -9732,7 +9731,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="233" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>8</v>
       </c>
@@ -9764,7 +9763,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="234" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>8</v>
       </c>
@@ -9796,7 +9795,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="235" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>8</v>
       </c>
@@ -9828,7 +9827,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="236" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>8</v>
       </c>
@@ -9860,7 +9859,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="237" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>8</v>
       </c>
@@ -9892,7 +9891,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="238" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>5</v>
       </c>
@@ -9924,7 +9923,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="239" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>6</v>
       </c>
@@ -9952,7 +9951,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="240" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>6</v>
       </c>
@@ -9980,7 +9979,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="241" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>6</v>
       </c>
@@ -10008,7 +10007,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="242" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>5</v>
       </c>
@@ -10040,7 +10039,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="243" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>5</v>
       </c>
@@ -10072,7 +10071,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="244" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>8</v>
       </c>
@@ -10104,7 +10103,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="245" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>8</v>
       </c>
@@ -10136,7 +10135,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="246" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>8</v>
       </c>
@@ -10168,7 +10167,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="247" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>8</v>
       </c>
@@ -10200,7 +10199,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="248" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>8</v>
       </c>
@@ -10232,7 +10231,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="249" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>8</v>
       </c>
@@ -10264,7 +10263,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="250" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>6</v>
       </c>
@@ -10292,7 +10291,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="251" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>5</v>
       </c>
@@ -10324,7 +10323,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="252" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>5</v>
       </c>
@@ -10356,7 +10355,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="253" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>5</v>
       </c>
@@ -10388,7 +10387,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="254" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>5</v>
       </c>
@@ -10420,7 +10419,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="255" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>5</v>
       </c>
@@ -10452,7 +10451,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="256" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>5</v>
       </c>
@@ -10484,7 +10483,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="257" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>5</v>
       </c>
@@ -10516,7 +10515,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="258" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>5</v>
       </c>
@@ -10548,7 +10547,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="259" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>5</v>
       </c>
@@ -10580,7 +10579,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="260" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>5</v>
       </c>
@@ -10612,7 +10611,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="261" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>5</v>
       </c>
@@ -10644,7 +10643,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="262" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>5</v>
       </c>
@@ -10676,7 +10675,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="263" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>5</v>
       </c>
@@ -10708,7 +10707,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="264" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>5</v>
       </c>
@@ -10740,7 +10739,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="265" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>5</v>
       </c>
@@ -10772,7 +10771,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="266" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>5</v>
       </c>
@@ -10804,7 +10803,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="267" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>8</v>
       </c>
@@ -10836,7 +10835,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="268" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>5</v>
       </c>
@@ -10869,13 +10868,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="I1:I268" xr:uid="{117D6E8E-35A8-4B5F-80FE-B0755FA1844B}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Recesos y Vacaciones"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="I1:I268" xr:uid="{117D6E8E-35A8-4B5F-80FE-B0755FA1844B}"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F5" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>#REF!</formula1>

</xml_diff>

<commit_message>
ya arregle las categorias y las buscar sin tildes y sin espacio
</commit_message>
<xml_diff>
--- a/excel/calendario-v1.xlsx
+++ b/excel/calendario-v1.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uredu-my.sharepoint.com/personal/luisfe_moreno_urosario_edu_co/Documents/calendario academico 2020 nuevo diseño/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{16003727-C6EF-4AB6-81B8-B898A4348C8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9D8AEA46-3F9F-4231-996F-AD43401C0DBB}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{16003727-C6EF-4AB6-81B8-B898A4348C8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6623D6CF-7B46-4BAC-8C33-D21FDF616DF9}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actividades" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Actividades!$I$1:$I$268</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Actividades!$A$1:$E$268</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -2554,10 +2554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:S268"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I130" sqref="I130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2610,7 +2611,7 @@
       </c>
       <c r="S1" s="18"/>
     </row>
-    <row r="2" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2639,7 +2640,7 @@
       </c>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -2668,7 +2669,7 @@
       </c>
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2695,7 +2696,7 @@
       <c r="J4" s="4"/>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2723,7 +2724,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -2751,7 +2752,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -2779,7 +2780,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2807,7 +2808,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -2835,7 +2836,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -2863,7 +2864,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -2895,7 +2896,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -2927,7 +2928,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
@@ -2959,7 +2960,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -2991,7 +2992,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
@@ -3023,7 +3024,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
@@ -3055,7 +3056,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -3087,7 +3088,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>5</v>
       </c>
@@ -3147,7 +3148,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>4</v>
       </c>
@@ -3175,7 +3176,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
@@ -3259,7 +3260,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>4</v>
       </c>
@@ -3287,7 +3288,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>4</v>
       </c>
@@ -3343,7 +3344,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>4</v>
       </c>
@@ -3371,7 +3372,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>4</v>
       </c>
@@ -3455,7 +3456,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>4</v>
       </c>
@@ -3511,7 +3512,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>4</v>
       </c>
@@ -3539,7 +3540,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>4</v>
       </c>
@@ -3567,7 +3568,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>4</v>
       </c>
@@ -3651,7 +3652,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>4</v>
       </c>
@@ -3679,7 +3680,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>4</v>
       </c>
@@ -3707,7 +3708,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>4</v>
       </c>
@@ -3735,7 +3736,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>4</v>
       </c>
@@ -3763,7 +3764,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>4</v>
       </c>
@@ -3791,7 +3792,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>4</v>
       </c>
@@ -3819,7 +3820,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>7</v>
       </c>
@@ -3851,7 +3852,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>7</v>
       </c>
@@ -3883,7 +3884,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>5</v>
       </c>
@@ -3915,7 +3916,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>5</v>
       </c>
@@ -3947,7 +3948,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>5</v>
       </c>
@@ -3979,7 +3980,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>5</v>
       </c>
@@ -4011,7 +4012,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>8</v>
       </c>
@@ -4043,7 +4044,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>8</v>
       </c>
@@ -4075,7 +4076,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>5</v>
       </c>
@@ -4107,7 +4108,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>5</v>
       </c>
@@ -4139,7 +4140,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>8</v>
       </c>
@@ -4171,7 +4172,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>8</v>
       </c>
@@ -4203,7 +4204,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>5</v>
       </c>
@@ -4235,7 +4236,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>5</v>
       </c>
@@ -4267,7 +4268,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>5</v>
       </c>
@@ -4299,7 +4300,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>5</v>
       </c>
@@ -4331,7 +4332,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>5</v>
       </c>
@@ -4363,7 +4364,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>5</v>
       </c>
@@ -4395,7 +4396,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>5</v>
       </c>
@@ -4427,7 +4428,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>5</v>
       </c>
@@ -4459,7 +4460,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>5</v>
       </c>
@@ -4491,7 +4492,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>5</v>
       </c>
@@ -4523,7 +4524,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>5</v>
       </c>
@@ -4555,7 +4556,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>4</v>
       </c>
@@ -4583,7 +4584,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>4</v>
       </c>
@@ -4611,7 +4612,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>4</v>
       </c>
@@ -4639,7 +4640,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>5</v>
       </c>
@@ -4671,7 +4672,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>5</v>
       </c>
@@ -4703,7 +4704,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>5</v>
       </c>
@@ -4735,7 +4736,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>5</v>
       </c>
@@ -4767,7 +4768,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>5</v>
       </c>
@@ -4799,7 +4800,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>5</v>
       </c>
@@ -4831,7 +4832,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>5</v>
       </c>
@@ -4863,7 +4864,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>5</v>
       </c>
@@ -4895,7 +4896,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>5</v>
       </c>
@@ -4927,7 +4928,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>8</v>
       </c>
@@ -4959,7 +4960,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>5</v>
       </c>
@@ -4991,7 +4992,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>8</v>
       </c>
@@ -5023,7 +5024,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>5</v>
       </c>
@@ -5055,7 +5056,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>5</v>
       </c>
@@ -5087,7 +5088,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>5</v>
       </c>
@@ -5119,7 +5120,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>8</v>
       </c>
@@ -5151,7 +5152,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>5</v>
       </c>
@@ -5183,7 +5184,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>8</v>
       </c>
@@ -5215,7 +5216,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>8</v>
       </c>
@@ -5247,7 +5248,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>8</v>
       </c>
@@ -5279,7 +5280,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>8</v>
       </c>
@@ -5311,7 +5312,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>8</v>
       </c>
@@ -5343,7 +5344,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>8</v>
       </c>
@@ -5375,7 +5376,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>8</v>
       </c>
@@ -5407,7 +5408,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>8</v>
       </c>
@@ -5439,7 +5440,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>8</v>
       </c>
@@ -5471,7 +5472,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>8</v>
       </c>
@@ -5503,7 +5504,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>8</v>
       </c>
@@ -5535,7 +5536,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>5</v>
       </c>
@@ -5567,7 +5568,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>5</v>
       </c>
@@ -5599,7 +5600,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>5</v>
       </c>
@@ -5631,7 +5632,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>5</v>
       </c>
@@ -5663,7 +5664,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>5</v>
       </c>
@@ -5695,7 +5696,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>5</v>
       </c>
@@ -5727,7 +5728,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>5</v>
       </c>
@@ -5759,7 +5760,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>4</v>
       </c>
@@ -5787,7 +5788,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>5</v>
       </c>
@@ -5819,7 +5820,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>4</v>
       </c>
@@ -5847,7 +5848,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>5</v>
       </c>
@@ -5879,7 +5880,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>5</v>
       </c>
@@ -5911,7 +5912,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>5</v>
       </c>
@@ -5943,7 +5944,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>5</v>
       </c>
@@ -5975,7 +5976,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>5</v>
       </c>
@@ -6007,7 +6008,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>5</v>
       </c>
@@ -6039,7 +6040,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>9</v>
       </c>
@@ -6067,7 +6068,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>9</v>
       </c>
@@ -6095,7 +6096,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>9</v>
       </c>
@@ -6123,7 +6124,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>9</v>
       </c>
@@ -6151,7 +6152,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>9</v>
       </c>
@@ -6179,7 +6180,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>9</v>
       </c>
@@ -6207,7 +6208,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>9</v>
       </c>
@@ -6235,7 +6236,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>9</v>
       </c>
@@ -6263,7 +6264,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>9</v>
       </c>
@@ -6291,7 +6292,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>9</v>
       </c>
@@ -6319,7 +6320,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>5</v>
       </c>
@@ -6351,7 +6352,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>9</v>
       </c>
@@ -6379,7 +6380,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>9</v>
       </c>
@@ -6407,7 +6408,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>9</v>
       </c>
@@ -6435,7 +6436,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>9</v>
       </c>
@@ -6463,7 +6464,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>9</v>
       </c>
@@ -6491,7 +6492,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>9</v>
       </c>
@@ -6519,7 +6520,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>9</v>
       </c>
@@ -6547,7 +6548,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>9</v>
       </c>
@@ -6575,7 +6576,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>9</v>
       </c>
@@ -6603,7 +6604,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>7</v>
       </c>
@@ -6635,7 +6636,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>4</v>
       </c>
@@ -6663,7 +6664,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>7</v>
       </c>
@@ -6695,7 +6696,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>7</v>
       </c>
@@ -6727,7 +6728,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>4</v>
       </c>
@@ -6755,7 +6756,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>7</v>
       </c>
@@ -6815,7 +6816,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>7</v>
       </c>
@@ -6875,7 +6876,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>7</v>
       </c>
@@ -6907,7 +6908,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>7</v>
       </c>
@@ -6967,7 +6968,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>5</v>
       </c>
@@ -6999,7 +7000,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>8</v>
       </c>
@@ -7031,7 +7032,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>8</v>
       </c>
@@ -7063,7 +7064,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>8</v>
       </c>
@@ -7095,7 +7096,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>8</v>
       </c>
@@ -7127,7 +7128,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>5</v>
       </c>
@@ -7159,7 +7160,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>5</v>
       </c>
@@ -7191,7 +7192,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>8</v>
       </c>
@@ -7223,7 +7224,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>8</v>
       </c>
@@ -7255,7 +7256,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>8</v>
       </c>
@@ -7287,7 +7288,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>8</v>
       </c>
@@ -7319,7 +7320,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>8</v>
       </c>
@@ -7351,7 +7352,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>8</v>
       </c>
@@ -7383,7 +7384,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>8</v>
       </c>
@@ -7415,7 +7416,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>5</v>
       </c>
@@ -7447,7 +7448,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>5</v>
       </c>
@@ -7479,7 +7480,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>5</v>
       </c>
@@ -7511,7 +7512,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>8</v>
       </c>
@@ -7543,7 +7544,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>8</v>
       </c>
@@ -7575,7 +7576,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>8</v>
       </c>
@@ -7607,7 +7608,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>8</v>
       </c>
@@ -7639,7 +7640,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>8</v>
       </c>
@@ -7671,7 +7672,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>5</v>
       </c>
@@ -7703,7 +7704,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>5</v>
       </c>
@@ -7735,7 +7736,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>5</v>
       </c>
@@ -7767,7 +7768,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>5</v>
       </c>
@@ -7799,7 +7800,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>5</v>
       </c>
@@ -7831,7 +7832,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>5</v>
       </c>
@@ -7863,7 +7864,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>5</v>
       </c>
@@ -7895,7 +7896,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>5</v>
       </c>
@@ -7927,7 +7928,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>5</v>
       </c>
@@ -7959,7 +7960,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>5</v>
       </c>
@@ -7991,7 +7992,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>5</v>
       </c>
@@ -8023,7 +8024,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>5</v>
       </c>
@@ -8055,7 +8056,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>8</v>
       </c>
@@ -8087,7 +8088,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>5</v>
       </c>
@@ -8119,7 +8120,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>5</v>
       </c>
@@ -8151,7 +8152,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>8</v>
       </c>
@@ -8183,7 +8184,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>5</v>
       </c>
@@ -8215,7 +8216,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>5</v>
       </c>
@@ -8247,7 +8248,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>5</v>
       </c>
@@ -8279,7 +8280,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>5</v>
       </c>
@@ -8367,7 +8368,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>5</v>
       </c>
@@ -8399,7 +8400,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>5</v>
       </c>
@@ -8431,7 +8432,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>5</v>
       </c>
@@ -8463,7 +8464,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>5</v>
       </c>
@@ -8495,7 +8496,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>5</v>
       </c>
@@ -8527,7 +8528,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>5</v>
       </c>
@@ -8559,7 +8560,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>5</v>
       </c>
@@ -8591,7 +8592,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>5</v>
       </c>
@@ -8623,7 +8624,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>5</v>
       </c>
@@ -8739,7 +8740,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>5</v>
       </c>
@@ -8771,7 +8772,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>5</v>
       </c>
@@ -8803,7 +8804,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>5</v>
       </c>
@@ -8835,7 +8836,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>5</v>
       </c>
@@ -8867,7 +8868,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>5</v>
       </c>
@@ -8899,7 +8900,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>5</v>
       </c>
@@ -8931,7 +8932,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>5</v>
       </c>
@@ -8963,7 +8964,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>5</v>
       </c>
@@ -8995,7 +8996,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>5</v>
       </c>
@@ -9027,7 +9028,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>5</v>
       </c>
@@ -9059,7 +9060,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>5</v>
       </c>
@@ -9091,7 +9092,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>5</v>
       </c>
@@ -9123,7 +9124,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>5</v>
       </c>
@@ -9155,7 +9156,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>5</v>
       </c>
@@ -9187,7 +9188,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>8</v>
       </c>
@@ -9219,7 +9220,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>8</v>
       </c>
@@ -9251,7 +9252,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>8</v>
       </c>
@@ -9283,7 +9284,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>8</v>
       </c>
@@ -9315,7 +9316,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>8</v>
       </c>
@@ -9347,7 +9348,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>8</v>
       </c>
@@ -9379,7 +9380,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>8</v>
       </c>
@@ -9411,7 +9412,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>5</v>
       </c>
@@ -9443,7 +9444,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>5</v>
       </c>
@@ -9475,7 +9476,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>5</v>
       </c>
@@ -9507,7 +9508,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>5</v>
       </c>
@@ -9539,7 +9540,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>5</v>
       </c>
@@ -9571,7 +9572,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>8</v>
       </c>
@@ -9603,7 +9604,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>10</v>
       </c>
@@ -9635,7 +9636,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>8</v>
       </c>
@@ -9667,7 +9668,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>8</v>
       </c>
@@ -9699,7 +9700,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>8</v>
       </c>
@@ -9731,7 +9732,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>8</v>
       </c>
@@ -9763,7 +9764,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>8</v>
       </c>
@@ -9795,7 +9796,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>8</v>
       </c>
@@ -9827,7 +9828,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>8</v>
       </c>
@@ -9859,7 +9860,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>8</v>
       </c>
@@ -9891,7 +9892,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>5</v>
       </c>
@@ -10007,7 +10008,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>5</v>
       </c>
@@ -10039,7 +10040,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>5</v>
       </c>
@@ -10071,7 +10072,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>8</v>
       </c>
@@ -10103,7 +10104,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>8</v>
       </c>
@@ -10135,7 +10136,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>8</v>
       </c>
@@ -10167,7 +10168,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>8</v>
       </c>
@@ -10199,7 +10200,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>8</v>
       </c>
@@ -10231,7 +10232,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>8</v>
       </c>
@@ -10291,7 +10292,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>5</v>
       </c>
@@ -10323,7 +10324,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>5</v>
       </c>
@@ -10355,7 +10356,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>5</v>
       </c>
@@ -10387,7 +10388,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>5</v>
       </c>
@@ -10419,7 +10420,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>5</v>
       </c>
@@ -10451,7 +10452,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>5</v>
       </c>
@@ -10483,7 +10484,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>5</v>
       </c>
@@ -10515,7 +10516,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>5</v>
       </c>
@@ -10547,7 +10548,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>5</v>
       </c>
@@ -10579,7 +10580,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>5</v>
       </c>
@@ -10611,7 +10612,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>5</v>
       </c>
@@ -10643,7 +10644,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>5</v>
       </c>
@@ -10675,7 +10676,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>5</v>
       </c>
@@ -10707,7 +10708,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>5</v>
       </c>
@@ -10739,7 +10740,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>5</v>
       </c>
@@ -10771,7 +10772,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>5</v>
       </c>
@@ -10803,7 +10804,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>8</v>
       </c>
@@ -10835,7 +10836,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>5</v>
       </c>
@@ -10868,7 +10869,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="I1:I268" xr:uid="{117D6E8E-35A8-4B5F-80FE-B0755FA1844B}"/>
+  <autoFilter ref="A1:E268" xr:uid="{1204C5BC-4CCB-4ED4-B4C5-04259704191C}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Funcionario"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F5" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>#REF!</formula1>

</xml_diff>